<commit_message>
informatiemodellen in hoofdmenu toegevoegd
</commit_message>
<xml_diff>
--- a/catalogusdata/matrix functionaliteit kenniskluis.xlsx
+++ b/catalogusdata/matrix functionaliteit kenniskluis.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="57">
   <si>
     <t>Concepten</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>getest in datasets/Begrippen BAG</t>
+  </si>
+  <si>
+    <t>Informatiemodellen</t>
   </si>
 </sst>
 </file>
@@ -563,17 +566,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O65"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D64" sqref="D64"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.44140625" bestFit="1" customWidth="1"/>
@@ -1180,7 +1183,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1188,103 +1191,103 @@
         <v>43</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
+      <c r="K37" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2" t="s">
-        <v>48</v>
-      </c>
+      <c r="A38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="8" t="s">
         <v>43</v>
@@ -1293,47 +1296,45 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="K38" s="2"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="B39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="2"/>
       <c r="D39" s="8" t="s">
         <v>43</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
+      <c r="K39" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2" t="s">
-        <v>55</v>
+      <c r="H40" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -1343,7 +1344,7 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>55</v>
@@ -1362,7 +1363,7 @@
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>55</v>
@@ -1381,7 +1382,7 @@
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>55</v>
@@ -1400,7 +1401,7 @@
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>55</v>
@@ -1418,20 +1419,24 @@
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
+      <c r="H45" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -1444,14 +1449,12 @@
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A47" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -1463,7 +1466,7 @@
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="8" t="s">
@@ -1480,7 +1483,7 @@
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="8" t="s">
@@ -1497,7 +1500,7 @@
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="8" t="s">
@@ -1512,12 +1515,14 @@
       <c r="K50" s="2"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B51" s="2"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="D51" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -1527,14 +1532,12 @@
       <c r="K51" s="2"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="A52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -1546,7 +1549,7 @@
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="8" t="s">
@@ -1561,12 +1564,14 @@
       <c r="K53" s="2"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="2"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="D54" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -1576,36 +1581,24 @@
       <c r="K54" s="2"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-      <c r="I55" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="I55" s="2"/>
       <c r="J55" s="2"/>
-      <c r="K55" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="K55" s="2"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="8" t="s">
@@ -1632,7 +1625,7 @@
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="8" t="s">
@@ -1659,7 +1652,7 @@
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="8" t="s">
@@ -1685,8 +1678,8 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
-      <c r="B59" s="3" t="s">
-        <v>24</v>
+      <c r="B59" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="8" t="s">
@@ -1713,7 +1706,7 @@
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="8" t="s">
@@ -1738,25 +1731,37 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="2"/>
+      <c r="B61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="2"/>
-      <c r="B62" s="3" t="s">
-        <v>27</v>
-      </c>
+      <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -1770,26 +1775,22 @@
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C63" s="2"/>
-      <c r="D63" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
-      <c r="I63" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2" t="s">
@@ -1806,21 +1807,40 @@
       <c r="K64" s="2"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="2"/>
+      <c r="B65" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="J65" s="2"/>
+      <c r="K65" s="2"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K65" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>